<commit_message>
EPBDS-9729 add more tests for different table types
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Strings_textSplit.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Strings_textSplit.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-pub\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\9683_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F51734-6C27-4422-89B4-943BF13AAA0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485CB534-BC1F-4500-8F16-8B06E6D1D062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="27855" windowHeight="14610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="174">
   <si>
     <t>Steps</t>
   </si>
@@ -214,13 +223,346 @@
   </si>
   <si>
     <t>_res_.$Case14</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult TestSplit ()</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>=textSplit(" ", "A software activation key is a string of letters and or numbers used to register or activate a software application. You may receive an activation key when you purchase a commercial software program")</t>
+  </si>
+  <si>
+    <t>2d</t>
+  </si>
+  <si>
+    <t>=textSplit(" ", " ")</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>=length($1st)</t>
+  </si>
+  <si>
+    <t>4th</t>
+  </si>
+  <si>
+    <t>=length($2d)</t>
+  </si>
+  <si>
+    <t>5th</t>
+  </si>
+  <si>
+    <t>6th</t>
+  </si>
+  <si>
+    <t>=$5th[0]</t>
+  </si>
+  <si>
+    <t>7th</t>
+  </si>
+  <si>
+    <t>=textSplit("/ ","abc/ def/ xyz")</t>
+  </si>
+  <si>
+    <t>8th</t>
+  </si>
+  <si>
+    <t>=$7th[0]</t>
+  </si>
+  <si>
+    <t>9th</t>
+  </si>
+  <si>
+    <t>=textSplit("* ","abc4/5* de!@#$%_-=;'frt^7&amp;()* xyz")</t>
+  </si>
+  <si>
+    <t>10th</t>
+  </si>
+  <si>
+    <t>=length($9th)</t>
+  </si>
+  <si>
+    <t>11th</t>
+  </si>
+  <si>
+    <t>=$9th[1]</t>
+  </si>
+  <si>
+    <t>12th</t>
+  </si>
+  <si>
+    <t>=textSplit("$ ","abc$ def$ xyz")</t>
+  </si>
+  <si>
+    <t>13th</t>
+  </si>
+  <si>
+    <t>=length($12th)</t>
+  </si>
+  <si>
+    <t>14th</t>
+  </si>
+  <si>
+    <t>=textSplit("' ", "abc' def' xyz")</t>
+  </si>
+  <si>
+    <t>Test   TestSplit  TestSplitTest</t>
+  </si>
+  <si>
+    <t>_res_.$1st</t>
+  </si>
+  <si>
+    <t>A, software, activation, key, is, a, string, of, letters, and, or, numbers, used, to, register, or, activate, a, software, application., You, may, receive, an, activation, key, when, you, purchase, a, commercial, software, program</t>
+  </si>
+  <si>
+    <t>_res_.$2d</t>
+  </si>
+  <si>
+    <t>_res_.$3d</t>
+  </si>
+  <si>
+    <t>_res_.$4th</t>
+  </si>
+  <si>
+    <t>_res_.$5th</t>
+  </si>
+  <si>
+    <t>abc,def,xyz</t>
+  </si>
+  <si>
+    <t>_res_.$6th</t>
+  </si>
+  <si>
+    <t>_res_.$7th</t>
+  </si>
+  <si>
+    <t>_res_.$8th</t>
+  </si>
+  <si>
+    <t>_res_.$9th</t>
+  </si>
+  <si>
+    <t>abc4/5,de!@#$%_-=;'frt^7&amp;(),xyz</t>
+  </si>
+  <si>
+    <t>_res_.$10th</t>
+  </si>
+  <si>
+    <t>_res_.$11th</t>
+  </si>
+  <si>
+    <t>de!@#$%_-=;'frt^7&amp;()</t>
+  </si>
+  <si>
+    <t>_res_.$12th</t>
+  </si>
+  <si>
+    <t>_res_.$13th</t>
+  </si>
+  <si>
+    <t>_res_.$14th</t>
+  </si>
+  <si>
+    <t>Tests with special symbols in a spreadsheet</t>
+  </si>
+  <si>
+    <t>Tests with Rules Tables</t>
+  </si>
+  <si>
+    <t>SmartRules String[] Splittest1 (Person person)</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>TaxValue</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>=textSplit(" ", name)</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>=textSplit("? ", name)</t>
+  </si>
+  <si>
+    <t>Test  Splittest1  Splittest1Test</t>
+  </si>
+  <si>
+    <t>person.name</t>
+  </si>
+  <si>
+    <t>person.gender</t>
+  </si>
+  <si>
+    <t>person.monthlySalary</t>
+  </si>
+  <si>
+    <t>person.age</t>
+  </si>
+  <si>
+    <t>person.children</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>ted tty tuu tutu gjgj gjj</t>
+  </si>
+  <si>
+    <t>ted, tty, tuu, tutu, gjgj, gjj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane? ryy? ryry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane, ryy, ryry </t>
+  </si>
+  <si>
+    <t>Rules String [] Splitrules(Person person)</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>length (textSplit(" ", name))</t>
+  </si>
+  <si>
+    <t>textSplit("+", param)</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>String param</t>
+  </si>
+  <si>
+    <t>Namelength</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>a+b+c</t>
+  </si>
+  <si>
+    <t>a+b+c+d</t>
+  </si>
+  <si>
+    <t>a+b+c+d+e</t>
+  </si>
+  <si>
+    <t>a+b+c+d+e+f</t>
+  </si>
+  <si>
+    <t>Test  Splitrules SplitrulesTest</t>
+  </si>
+  <si>
+    <t>ted tty tuu tutu</t>
+  </si>
+  <si>
+    <t>a, b, c, d, e, f</t>
+  </si>
+  <si>
+    <t>jane ryy</t>
+  </si>
+  <si>
+    <t>a, b, c, d</t>
+  </si>
+  <si>
+    <t>Tests with Rules Tables with External condition</t>
+  </si>
+  <si>
+    <t>SmartRules String[] SplitrulesEx (Person person)</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Returns</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Person person</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Test  SplitrulesEx SplitrulesExTest</t>
+  </si>
+  <si>
+    <t>Datatype Person</t>
+  </si>
+  <si>
+    <t>Datatype Gender &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender </t>
+  </si>
+  <si>
+    <t>monthlySalary</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Person []</t>
+  </si>
+  <si>
+    <t>ABc,def,Xyz</t>
+  </si>
+  <si>
+    <t>=textSplit("? ","ABc? def? Xyz")</t>
+  </si>
+  <si>
+    <t>ABc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,16 +570,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -245,19 +619,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3 2" xfId="1" xr:uid="{5E398044-84C7-4A85-AF40-4A1B731A5F3E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -535,34 +940,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C6:J24"/>
+  <dimension ref="B6:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="53.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="53.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="D6" s="6"/>
+      <c r="H6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>0</v>
       </c>
@@ -576,7 +981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>2</v>
       </c>
@@ -588,7 +993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>3</v>
       </c>
@@ -602,7 +1007,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>5</v>
       </c>
@@ -616,7 +1021,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>7</v>
       </c>
@@ -633,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>8</v>
       </c>
@@ -650,7 +1055,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -667,7 +1072,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>31</v>
       </c>
@@ -684,7 +1089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>12</v>
       </c>
@@ -701,7 +1106,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>33</v>
       </c>
@@ -718,7 +1123,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>13</v>
       </c>
@@ -735,7 +1140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -752,7 +1157,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>41</v>
       </c>
@@ -769,7 +1174,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>44</v>
       </c>
@@ -786,7 +1191,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>49</v>
       </c>
@@ -803,7 +1208,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>51</v>
       </c>
@@ -820,7 +1225,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>55</v>
       </c>
@@ -837,12 +1242,694 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>59</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32" t="s">
+        <v>93</v>
+      </c>
+      <c r="J32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" t="s">
+        <v>95</v>
+      </c>
+      <c r="I33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" t="s">
+        <v>96</v>
+      </c>
+      <c r="I34" t="s">
+        <v>96</v>
+      </c>
+      <c r="J34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+      <c r="H35" t="s">
+        <v>97</v>
+      </c>
+      <c r="I35" t="s">
+        <v>97</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" t="s">
+        <v>98</v>
+      </c>
+      <c r="I36" t="s">
+        <v>98</v>
+      </c>
+      <c r="J36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="H37" t="s">
+        <v>100</v>
+      </c>
+      <c r="I37" t="s">
+        <v>100</v>
+      </c>
+      <c r="J37" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" t="s">
+        <v>101</v>
+      </c>
+      <c r="I38" t="s">
+        <v>101</v>
+      </c>
+      <c r="J38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" t="s">
+        <v>102</v>
+      </c>
+      <c r="I39" t="s">
+        <v>102</v>
+      </c>
+      <c r="J39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" t="s">
+        <v>79</v>
+      </c>
+      <c r="H40" t="s">
+        <v>103</v>
+      </c>
+      <c r="I40" t="s">
+        <v>103</v>
+      </c>
+      <c r="J40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" t="s">
+        <v>81</v>
+      </c>
+      <c r="H41" t="s">
+        <v>105</v>
+      </c>
+      <c r="I41" t="s">
+        <v>105</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" t="s">
+        <v>106</v>
+      </c>
+      <c r="I42" t="s">
+        <v>106</v>
+      </c>
+      <c r="J42" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" t="s">
+        <v>108</v>
+      </c>
+      <c r="I43" t="s">
+        <v>108</v>
+      </c>
+      <c r="J43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+      <c r="D44" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" t="s">
+        <v>109</v>
+      </c>
+      <c r="I44" t="s">
+        <v>109</v>
+      </c>
+      <c r="J44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" t="s">
+        <v>89</v>
+      </c>
+      <c r="H45" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" t="s">
+        <v>110</v>
+      </c>
+      <c r="J45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+      <c r="D46" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" t="s">
+        <v>121</v>
+      </c>
+      <c r="F53" t="s">
+        <v>122</v>
+      </c>
+      <c r="G53" t="s">
+        <v>123</v>
+      </c>
+      <c r="H53" t="s">
+        <v>124</v>
+      </c>
+      <c r="I53" t="s">
+        <v>125</v>
+      </c>
+      <c r="J53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" t="s">
+        <v>127</v>
+      </c>
+      <c r="F54" t="s">
+        <v>128</v>
+      </c>
+      <c r="G54" t="s">
+        <v>129</v>
+      </c>
+      <c r="H54" t="s">
+        <v>130</v>
+      </c>
+      <c r="I54" t="s">
+        <v>131</v>
+      </c>
+      <c r="J54" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" t="s">
+        <v>119</v>
+      </c>
+      <c r="E55" t="s">
+        <v>132</v>
+      </c>
+      <c r="F55" t="s">
+        <v>116</v>
+      </c>
+      <c r="G55">
+        <v>2000</v>
+      </c>
+      <c r="H55">
+        <v>30</v>
+      </c>
+      <c r="J55" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>134</v>
+      </c>
+      <c r="F56" t="s">
+        <v>118</v>
+      </c>
+      <c r="G56">
+        <v>3000</v>
+      </c>
+      <c r="H56">
+        <v>30</v>
+      </c>
+      <c r="J56" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" t="s">
+        <v>138</v>
+      </c>
+      <c r="E60" t="s">
+        <v>121</v>
+      </c>
+      <c r="F60" t="s">
+        <v>122</v>
+      </c>
+      <c r="G60" t="s">
+        <v>123</v>
+      </c>
+      <c r="H60" t="s">
+        <v>124</v>
+      </c>
+      <c r="I60" t="s">
+        <v>125</v>
+      </c>
+      <c r="J60" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>139</v>
+      </c>
+      <c r="C61" t="s">
+        <v>140</v>
+      </c>
+      <c r="E61" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" t="s">
+        <v>128</v>
+      </c>
+      <c r="G61" t="s">
+        <v>129</v>
+      </c>
+      <c r="H61" t="s">
+        <v>130</v>
+      </c>
+      <c r="I61" t="s">
+        <v>131</v>
+      </c>
+      <c r="J61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>141</v>
+      </c>
+      <c r="C62" t="s">
+        <v>142</v>
+      </c>
+      <c r="E62" t="s">
+        <v>150</v>
+      </c>
+      <c r="F62" t="s">
+        <v>116</v>
+      </c>
+      <c r="G62">
+        <v>2000</v>
+      </c>
+      <c r="H62">
+        <v>30</v>
+      </c>
+      <c r="J62" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" t="s">
+        <v>144</v>
+      </c>
+      <c r="E63" t="s">
+        <v>152</v>
+      </c>
+      <c r="F63" t="s">
+        <v>118</v>
+      </c>
+      <c r="G63">
+        <v>3000</v>
+      </c>
+      <c r="H63">
+        <v>30</v>
+      </c>
+      <c r="J63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>155</v>
+      </c>
+      <c r="E73" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" t="s">
+        <v>144</v>
+      </c>
+      <c r="E74" t="s">
+        <v>121</v>
+      </c>
+      <c r="F74" t="s">
+        <v>122</v>
+      </c>
+      <c r="G74" t="s">
+        <v>123</v>
+      </c>
+      <c r="H74" t="s">
+        <v>124</v>
+      </c>
+      <c r="I74" t="s">
+        <v>125</v>
+      </c>
+      <c r="J74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>145</v>
+      </c>
+      <c r="E75" t="s">
+        <v>127</v>
+      </c>
+      <c r="F75" t="s">
+        <v>128</v>
+      </c>
+      <c r="G75" t="s">
+        <v>129</v>
+      </c>
+      <c r="H75" t="s">
+        <v>130</v>
+      </c>
+      <c r="I75" t="s">
+        <v>131</v>
+      </c>
+      <c r="J75" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76" t="s">
+        <v>146</v>
+      </c>
+      <c r="E76" t="s">
+        <v>150</v>
+      </c>
+      <c r="F76" t="s">
+        <v>116</v>
+      </c>
+      <c r="G76">
+        <v>2000</v>
+      </c>
+      <c r="H76">
+        <v>30</v>
+      </c>
+      <c r="J76" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77" t="s">
+        <v>147</v>
+      </c>
+      <c r="E77" t="s">
+        <v>152</v>
+      </c>
+      <c r="F77" t="s">
+        <v>118</v>
+      </c>
+      <c r="G77">
+        <v>3000</v>
+      </c>
+      <c r="H77">
+        <v>30</v>
+      </c>
+      <c r="J77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>156</v>
+      </c>
+      <c r="E81" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" t="s">
+        <v>159</v>
+      </c>
+      <c r="E82" t="s">
+        <v>158</v>
+      </c>
+      <c r="F82" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>160</v>
+      </c>
+      <c r="C83" t="s">
+        <v>139</v>
+      </c>
+      <c r="E83" t="s">
+        <v>160</v>
+      </c>
+      <c r="F83" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" t="s">
+        <v>141</v>
+      </c>
+      <c r="E84" t="s">
+        <v>161</v>
+      </c>
+      <c r="F84" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" t="s">
+        <v>143</v>
+      </c>
+      <c r="E85" t="s">
+        <v>162</v>
+      </c>
+      <c r="F85" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -853,4 +1940,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1D372EE-5AF2-422B-8481-26285BC7F58C}">
+  <dimension ref="B3:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="E3" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>